<commit_message>
chore: update faculty and major data in Excel files
</commit_message>
<xml_diff>
--- a/src/seeders/files/xlsx/faculties.xlsx
+++ b/src/seeders/files/xlsx/faculties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phinc\Documents\projects\phincon\personal_project\Project-Akreditasi\src\seeders\files\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\Project-Akreditasi\src\seeders\files\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5E315C-F7A7-47EE-84FB-7BAD5A458DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEE6375-2F03-40EF-A4A1-701F75EC239F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>code</t>
   </si>
@@ -40,6 +40,84 @@
   </si>
   <si>
     <t>General</t>
+  </si>
+  <si>
+    <t>Fakultas Ilmu Komputer dan Teknologi Informasi</t>
+  </si>
+  <si>
+    <t>FIKTI</t>
+  </si>
+  <si>
+    <t>FIKF</t>
+  </si>
+  <si>
+    <t>Fakultas Ilmu Kesehatan dan Farmasi</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>Fakultas Kedokteran</t>
+  </si>
+  <si>
+    <t>FTSP</t>
+  </si>
+  <si>
+    <t>Fakultas Teknik Sipil dan Perencanaan</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>Fakultas Ekonomi</t>
+  </si>
+  <si>
+    <t>FPSI</t>
+  </si>
+  <si>
+    <t>Fakultas Psikologi</t>
+  </si>
+  <si>
+    <t>FTI</t>
+  </si>
+  <si>
+    <t>Fakultas Teknologi Industri</t>
+  </si>
+  <si>
+    <t>FSB</t>
+  </si>
+  <si>
+    <t>Fakultas Sastra dan Budaya</t>
+  </si>
+  <si>
+    <t>FIKOM</t>
+  </si>
+  <si>
+    <t>Fakultas Ilmu Komunikasi</t>
+  </si>
+  <si>
+    <t>FTI_DIPLOMA</t>
+  </si>
+  <si>
+    <t>Fakultas Teknologi Informasi</t>
+  </si>
+  <si>
+    <t>FBK</t>
+  </si>
+  <si>
+    <t>Fakultas Bisnis dan Kewirausahaan</t>
+  </si>
+  <si>
+    <t>MAGISTER</t>
+  </si>
+  <si>
+    <t>Program Magister</t>
+  </si>
+  <si>
+    <t>PROFESI</t>
+  </si>
+  <si>
+    <t>Program Profesi</t>
   </si>
 </sst>
 </file>
@@ -357,20 +435,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,7 +459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -389,6 +467,149 @@
         <v>4</v>
       </c>
       <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>